<commit_message>
tentative phylgeny figures species preferences model results delay data added
</commit_message>
<xml_diff>
--- a/results/Supplementary/5. Species x incubator traits summary.xlsx
+++ b/results/Supplementary/5. Species x incubator traits summary.xlsx
@@ -1,27 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/movealong/results/Tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/movealong/results/Supplementary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="587" documentId="8_{A3E84667-6380-4BF0-9B62-CFD1E679C2F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E477E8F-B0DC-4463-84F0-9136533B6683}"/>
+  <xr:revisionPtr revIDLastSave="625" documentId="8_{A3E84667-6380-4BF0-9B62-CFD1E679C2F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE5EDD9D-DA44-421E-BCF1-4C4A4541C599}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="7335" yWindow="1140" windowWidth="13110" windowHeight="14805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Temperate" sheetId="1" r:id="rId1"/>
     <sheet name="Mediterranean" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="68">
   <si>
     <t>Agrostis tileni</t>
   </si>
@@ -219,6 +232,12 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>Delay time to 50% germ (days)</t>
+  </si>
+  <si>
+    <t>Time to reach 50% germination (days)</t>
   </si>
 </sst>
 </file>
@@ -545,7 +564,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -675,6 +694,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -720,7 +765,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -751,6 +796,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -815,10 +866,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1121,20 +1168,23 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="13" width="6.85546875" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="6.85546875" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" customWidth="1"/>
+    <col min="12" max="13" width="6.85546875" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>56</v>
       </c>
@@ -1155,18 +1205,21 @@
       </c>
       <c r="I1" s="11"/>
       <c r="J1" s="11" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="K1" s="11"/>
       <c r="L1" s="11" t="s">
         <v>61</v>
       </c>
       <c r="M1" s="11"/>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" s="10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="3" t="s">
         <v>64</v>
@@ -1204,9 +1257,10 @@
       <c r="M2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="N2" s="10"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N2" s="13"/>
+      <c r="O2" s="10"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>22</v>
       </c>
@@ -1246,11 +1300,14 @@
       <c r="M3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="5">
         <v>-0.63234170000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>23</v>
       </c>
@@ -1290,11 +1347,14 @@
       <c r="M4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="5">
         <v>12.15582</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>24</v>
       </c>
@@ -1334,11 +1394,14 @@
       <c r="M5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="5">
         <v>69.102739999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>25</v>
       </c>
@@ -1378,11 +1441,15 @@
       <c r="M6" s="2">
         <v>792</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="2">
+        <f t="shared" ref="N4:N39" si="0">K6-J6</f>
+        <v>22</v>
+      </c>
+      <c r="O6" s="5">
         <v>30.777899999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>26</v>
       </c>
@@ -1422,11 +1489,15 @@
       <c r="M7" s="2">
         <v>596.75</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="2">
+        <f t="shared" si="0"/>
+        <v>39.801388888888994</v>
+      </c>
+      <c r="O7" s="5">
         <v>30.845549999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
@@ -1466,11 +1537,15 @@
       <c r="M8" s="2">
         <v>548.3125</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="2">
+        <f t="shared" si="0"/>
+        <v>38.043102073364992</v>
+      </c>
+      <c r="O8" s="5">
         <v>38.153109999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>28</v>
       </c>
@@ -1510,11 +1585,15 @@
       <c r="M9" s="2">
         <v>251.875</v>
       </c>
-      <c r="N9" s="5">
+      <c r="N9" s="2">
+        <f t="shared" si="0"/>
+        <v>17.501092657343008</v>
+      </c>
+      <c r="O9" s="5">
         <v>11.870900000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>29</v>
       </c>
@@ -1554,11 +1633,15 @@
       <c r="M10" s="2">
         <v>325.125</v>
       </c>
-      <c r="N10" s="5">
+      <c r="N10" s="2">
+        <f t="shared" si="0"/>
+        <v>41.892647058824025</v>
+      </c>
+      <c r="O10" s="5">
         <v>43.796329999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>30</v>
       </c>
@@ -1598,11 +1681,14 @@
       <c r="M11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N11" s="5">
+      <c r="N11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O11" s="5">
         <v>7.7578389999999997E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>31</v>
       </c>
@@ -1642,11 +1728,15 @@
       <c r="M12" s="2">
         <v>178</v>
       </c>
-      <c r="N12" s="5">
+      <c r="N12" s="2">
+        <f t="shared" si="0"/>
+        <v>107.739583333333</v>
+      </c>
+      <c r="O12" s="5">
         <v>83.157409999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>32</v>
       </c>
@@ -1674,11 +1764,15 @@
         <v>648</v>
       </c>
       <c r="M13" s="2"/>
-      <c r="N13" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N13" s="2">
+        <f t="shared" si="0"/>
+        <v>-239.5</v>
+      </c>
+      <c r="O13" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>33</v>
       </c>
@@ -1718,11 +1812,14 @@
       <c r="M14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N14" s="5">
+      <c r="N14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O14" s="5">
         <v>1.2084980000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>34</v>
       </c>
@@ -1762,11 +1859,14 @@
       <c r="M15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N15" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O15" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>35</v>
       </c>
@@ -1806,11 +1906,15 @@
       <c r="M16" s="2">
         <v>523.125</v>
       </c>
-      <c r="N16" s="5">
+      <c r="N16" s="2">
+        <f t="shared" si="0"/>
+        <v>51.553265668154978</v>
+      </c>
+      <c r="O16" s="5">
         <v>75.370099999999994</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>36</v>
       </c>
@@ -1850,11 +1954,14 @@
       <c r="M17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N17" s="5">
+      <c r="N17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O17" s="5">
         <v>29.819759999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>37</v>
       </c>
@@ -1894,11 +2001,15 @@
       <c r="M18" s="2">
         <v>91</v>
       </c>
-      <c r="N18" s="5">
+      <c r="N18" s="2">
+        <f t="shared" si="0"/>
+        <v>1.4401041666666003</v>
+      </c>
+      <c r="O18" s="5">
         <v>-32.509419999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>38</v>
       </c>
@@ -1938,11 +2049,15 @@
       <c r="M19" s="2">
         <v>277</v>
       </c>
-      <c r="N19" s="5">
+      <c r="N19" s="2">
+        <f t="shared" si="0"/>
+        <v>2.0187500000000114</v>
+      </c>
+      <c r="O19" s="5">
         <v>23.03575</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>39</v>
       </c>
@@ -1982,11 +2097,15 @@
       <c r="M20" s="2">
         <v>1005.875</v>
       </c>
-      <c r="N20" s="5">
+      <c r="N20" s="2">
+        <f t="shared" si="0"/>
+        <v>302.11065423976595</v>
+      </c>
+      <c r="O20" s="5">
         <v>183.4111</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>40</v>
       </c>
@@ -2026,11 +2145,15 @@
       <c r="M21" s="2">
         <v>474.25</v>
       </c>
-      <c r="N21" s="5">
+      <c r="N21" s="2">
+        <f t="shared" si="0"/>
+        <v>46.041666666667027</v>
+      </c>
+      <c r="O21" s="5">
         <v>14.02195</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>7</v>
       </c>
@@ -2070,11 +2193,15 @@
       <c r="M22" s="2">
         <v>268.5</v>
       </c>
-      <c r="N22" s="5">
+      <c r="N22" s="2">
+        <f t="shared" si="0"/>
+        <v>110.916666666667</v>
+      </c>
+      <c r="O22" s="5">
         <v>94.146439999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>41</v>
       </c>
@@ -2114,11 +2241,14 @@
       <c r="M23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N23" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O23" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>42</v>
       </c>
@@ -2158,11 +2288,15 @@
       <c r="M24" s="2">
         <v>185.9375</v>
       </c>
-      <c r="N24" s="5">
+      <c r="N24" s="2">
+        <f t="shared" si="0"/>
+        <v>17.894845085470099</v>
+      </c>
+      <c r="O24" s="5">
         <v>54.54562</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>43</v>
       </c>
@@ -2202,11 +2336,14 @@
       <c r="M25" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N25" s="5">
+      <c r="N25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O25" s="5">
         <v>97.170490000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>44</v>
       </c>
@@ -2246,11 +2383,14 @@
       <c r="M26" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N26" s="5">
+      <c r="N26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O26" s="5">
         <v>112.3931</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>45</v>
       </c>
@@ -2290,11 +2430,15 @@
       <c r="M27" s="2">
         <v>334</v>
       </c>
-      <c r="N27" s="5">
+      <c r="N27" s="2">
+        <f t="shared" si="0"/>
+        <v>45.78333333333299</v>
+      </c>
+      <c r="O27" s="5">
         <v>21.053730000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>46</v>
       </c>
@@ -2334,11 +2478,14 @@
       <c r="M28" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N28" s="5">
+      <c r="N28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O28" s="5">
         <v>-11.422639999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>47</v>
       </c>
@@ -2378,11 +2525,15 @@
       <c r="M29" s="2">
         <v>225.333333333333</v>
       </c>
-      <c r="N29" s="5">
+      <c r="N29" s="2">
+        <f t="shared" si="0"/>
+        <v>58.515758547008005</v>
+      </c>
+      <c r="O29" s="5">
         <v>82.974209999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>48</v>
       </c>
@@ -2422,11 +2573,14 @@
       <c r="M30" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N30" s="5">
+      <c r="N30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O30" s="5">
         <v>24.668749999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>49</v>
       </c>
@@ -2464,11 +2618,14 @@
         <v>13</v>
       </c>
       <c r="M31" s="2"/>
-      <c r="N31" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O31" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>50</v>
       </c>
@@ -2508,11 +2665,15 @@
       <c r="M32" s="2">
         <v>1284.6666666666699</v>
       </c>
-      <c r="N32" s="5">
+      <c r="N32" s="2">
+        <f t="shared" si="0"/>
+        <v>265.06246565934072</v>
+      </c>
+      <c r="O32" s="5">
         <v>195.16929999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>51</v>
       </c>
@@ -2552,11 +2713,15 @@
       <c r="M33" s="2">
         <v>551.5</v>
       </c>
-      <c r="N33" s="5">
+      <c r="N33" s="2">
+        <f t="shared" si="0"/>
+        <v>61.502252700321975</v>
+      </c>
+      <c r="O33" s="5">
         <v>84.829350000000005</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>52</v>
       </c>
@@ -2596,11 +2761,14 @@
       <c r="M34" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N34" s="5">
+      <c r="N34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O34" s="5">
         <v>-1.361059</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>53</v>
       </c>
@@ -2640,11 +2808,14 @@
       <c r="M35" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N35" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O35" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>54</v>
       </c>
@@ -2684,11 +2855,15 @@
       <c r="M36" s="2">
         <v>304.625</v>
       </c>
-      <c r="N36" s="5">
+      <c r="N36" s="2">
+        <f t="shared" si="0"/>
+        <v>170.35584935897438</v>
+      </c>
+      <c r="O36" s="5">
         <v>146.8434</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>55</v>
       </c>
@@ -2728,11 +2903,15 @@
       <c r="M37" s="2">
         <v>692.5</v>
       </c>
-      <c r="N37" s="5">
+      <c r="N37" s="2">
+        <f t="shared" si="0"/>
+        <v>-15.916666666667027</v>
+      </c>
+      <c r="O37" s="5">
         <v>17.534929999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>18</v>
       </c>
@@ -2772,11 +2951,15 @@
       <c r="M38" s="2">
         <v>296.9375</v>
       </c>
-      <c r="N38" s="5">
+      <c r="N38" s="2">
+        <f t="shared" si="0"/>
+        <v>44.920833333332979</v>
+      </c>
+      <c r="O38" s="5">
         <v>56.58296</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>21</v>
       </c>
@@ -2816,13 +2999,17 @@
       <c r="M39" s="2">
         <v>459.1875</v>
       </c>
-      <c r="N39" s="5">
+      <c r="N39" s="2">
+        <f t="shared" si="0"/>
+        <v>153.20126902734796</v>
+      </c>
+      <c r="O39" s="5">
         <v>151.82660000000001</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="N1:N2"/>
+  <mergeCells count="9">
+    <mergeCell ref="O1:O2"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="A1:A2"/>
@@ -2830,6 +3017,7 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
+    <mergeCell ref="N1:N2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="82" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -2838,20 +3026,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39C9B01A-1797-44E2-A234-EAC5F2F58B98}">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="13" width="6.85546875" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" customWidth="1"/>
+    <col min="14" max="14" width="12" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>56</v>
       </c>
@@ -2879,11 +3068,14 @@
         <v>61</v>
       </c>
       <c r="M1" s="11"/>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" s="10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="9" t="s">
         <v>64</v>
@@ -2921,9 +3113,10 @@
       <c r="M2" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="N2" s="10"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N2" s="13"/>
+      <c r="O2" s="10"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -2963,11 +3156,15 @@
       <c r="M3" s="2">
         <v>817.5</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="2">
+        <f>K3-J3</f>
+        <v>76.208333333334025</v>
+      </c>
+      <c r="O3" s="5">
         <v>69.814580000000007</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -3007,11 +3204,15 @@
       <c r="M4" s="2">
         <v>130.9375</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="2">
+        <f t="shared" ref="N4:N23" si="0">K4-J4</f>
+        <v>7.9117797796215994</v>
+      </c>
+      <c r="O4" s="5">
         <v>25.44096</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -3051,11 +3252,15 @@
       <c r="M5" s="2">
         <v>755.625</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.78769363806129888</v>
+      </c>
+      <c r="O5" s="5">
         <v>-8.0269919999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -3095,11 +3300,15 @@
       <c r="M6" s="2">
         <v>354.25</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="2">
+        <f t="shared" si="0"/>
+        <v>31.404464285713999</v>
+      </c>
+      <c r="O6" s="5">
         <v>29.18449</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -3139,11 +3348,15 @@
       <c r="M7" s="2">
         <v>70.25</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="2">
+        <f t="shared" si="0"/>
+        <v>1.6747985793287596</v>
+      </c>
+      <c r="O7" s="5">
         <v>6.1222849999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -3183,11 +3396,15 @@
       <c r="M8" s="2">
         <v>182.25</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="2">
+        <f t="shared" si="0"/>
+        <v>4.7317833310481028</v>
+      </c>
+      <c r="O8" s="5">
         <v>17.046119999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -3227,11 +3444,15 @@
       <c r="M9" s="2">
         <v>432.5</v>
       </c>
-      <c r="N9" s="5">
+      <c r="N9" s="2">
+        <f t="shared" si="0"/>
+        <v>22.927083333333002</v>
+      </c>
+      <c r="O9" s="5">
         <v>34.588180000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -3271,11 +3492,15 @@
       <c r="M10" s="2">
         <v>445.5</v>
       </c>
-      <c r="N10" s="5">
+      <c r="N10" s="2">
+        <f t="shared" si="0"/>
+        <v>236.78958333333333</v>
+      </c>
+      <c r="O10" s="5">
         <v>191.21639999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -3315,11 +3540,15 @@
       <c r="M11" s="2">
         <v>432.5</v>
       </c>
-      <c r="N11" s="5">
+      <c r="N11" s="2">
+        <f t="shared" si="0"/>
+        <v>143.19742063491998</v>
+      </c>
+      <c r="O11" s="5">
         <v>107.0115</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
@@ -3359,11 +3588,15 @@
       <c r="M12" s="2">
         <v>159.75</v>
       </c>
-      <c r="N12" s="5">
+      <c r="N12" s="2">
+        <f t="shared" si="0"/>
+        <v>8.0281508513416604</v>
+      </c>
+      <c r="O12" s="5">
         <v>54.196770000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
@@ -3403,11 +3636,15 @@
       <c r="M13" s="2">
         <v>75.8125</v>
       </c>
-      <c r="N13" s="5">
+      <c r="N13" s="2">
+        <f t="shared" si="0"/>
+        <v>1.9837693910836407</v>
+      </c>
+      <c r="O13" s="5">
         <v>17.603860000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
@@ -3447,11 +3684,15 @@
       <c r="M14" s="2">
         <v>278.5625</v>
       </c>
-      <c r="N14" s="5">
+      <c r="N14" s="2">
+        <f t="shared" si="0"/>
+        <v>41.828593129960296</v>
+      </c>
+      <c r="O14" s="5">
         <v>2.7350300000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>12</v>
       </c>
@@ -3491,11 +3732,14 @@
       <c r="M15" s="2">
         <v>547</v>
       </c>
-      <c r="N15" s="5">
+      <c r="N15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O15" s="5">
         <v>10.14752</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
@@ -3535,11 +3779,15 @@
       <c r="M16" s="2">
         <v>71.4375</v>
       </c>
-      <c r="N16" s="5">
+      <c r="N16" s="2">
+        <f t="shared" si="0"/>
+        <v>0.31812005928853004</v>
+      </c>
+      <c r="O16" s="5">
         <v>8.8713510000000007</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
@@ -3579,11 +3827,15 @@
       <c r="M17" s="2">
         <v>515.1875</v>
       </c>
-      <c r="N17" s="5">
+      <c r="N17" s="2">
+        <f t="shared" si="0"/>
+        <v>82.447743055555705</v>
+      </c>
+      <c r="O17" s="5">
         <v>62.859369999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
@@ -3623,11 +3875,15 @@
       <c r="M18" s="2">
         <v>240.625</v>
       </c>
-      <c r="N18" s="5">
+      <c r="N18" s="2">
+        <f t="shared" si="0"/>
+        <v>9.8447802197801906</v>
+      </c>
+      <c r="O18" s="5">
         <v>28.353670000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
@@ -3667,11 +3923,15 @@
       <c r="M19" s="2">
         <v>351</v>
       </c>
-      <c r="N19" s="5">
+      <c r="N19" s="2">
+        <f t="shared" si="0"/>
+        <v>47.036849261848971</v>
+      </c>
+      <c r="O19" s="5">
         <v>55.334409999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
@@ -3711,11 +3971,15 @@
       <c r="M20" s="2">
         <v>184.375</v>
       </c>
-      <c r="N20" s="5">
+      <c r="N20" s="2">
+        <f t="shared" si="0"/>
+        <v>41.888991013071006</v>
+      </c>
+      <c r="O20" s="5">
         <v>30.549150000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>19</v>
       </c>
@@ -3755,11 +4019,15 @@
       <c r="M21" s="2">
         <v>305.5625</v>
       </c>
-      <c r="N21" s="5">
+      <c r="N21" s="2">
+        <f t="shared" si="0"/>
+        <v>220.3694991283221</v>
+      </c>
+      <c r="O21" s="5">
         <v>164.5787</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>20</v>
       </c>
@@ -3799,11 +4067,15 @@
       <c r="M22" s="2">
         <v>559.08333333333303</v>
       </c>
-      <c r="N22" s="5">
+      <c r="N22" s="2">
+        <f t="shared" si="0"/>
+        <v>-131.6736189431912</v>
+      </c>
+      <c r="O22" s="5">
         <v>-62.093020000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
@@ -3843,13 +4115,17 @@
       <c r="M23" s="2">
         <v>265.875</v>
       </c>
-      <c r="N23" s="5">
+      <c r="N23" s="2">
+        <f t="shared" si="0"/>
+        <v>69.544305398441395</v>
+      </c>
+      <c r="O23" s="5">
         <v>65.792850000000001</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="N1:N2"/>
+  <mergeCells count="9">
+    <mergeCell ref="O1:O2"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="L1:M1"/>
@@ -3857,6 +4133,7 @@
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="N1:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Figures and scripts updated manuscript with minor terms changes
</commit_message>
<xml_diff>
--- a/results/Supplementary/5. Species x incubator traits summary.xlsx
+++ b/results/Supplementary/5. Species x incubator traits summary.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/movealong/results/Supplementary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laptop\OneDrive - Universidad de Oviedo\IMIB\Softwares\GitHub\movealong\results\Supplementary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="625" documentId="8_{A3E84667-6380-4BF0-9B62-CFD1E679C2F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE5EDD9D-DA44-421E-BCF1-4C4A4541C599}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Temperate" sheetId="1" r:id="rId1"/>
@@ -243,7 +242,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -824,7 +823,7 @@
     <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Buena" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
@@ -1164,14 +1163,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1442,7 +1441,7 @@
         <v>792</v>
       </c>
       <c r="N6" s="2">
-        <f t="shared" ref="N4:N39" si="0">K6-J6</f>
+        <f t="shared" ref="N6:N39" si="0">K6-J6</f>
         <v>22</v>
       </c>
       <c r="O6" s="5">
@@ -3025,7 +3024,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39C9B01A-1797-44E2-A234-EAC5F2F58B98}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>